<commit_message>
Compute electrical, heat consumption and capacities of modules
</commit_message>
<xml_diff>
--- a/code/h2_tech.xlsx
+++ b/code/h2_tech.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/Library/CloudStorage/OneDrive-IdahoNationalLaboratory/Documents/Research/Hydrogen from Nuclear/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3154CC2E-32FE-9B40-AE72-455B1A5DA061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E3DF65-3AFA-204D-81BA-D88516691CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54940" yWindow="500" windowWidth="19180" windowHeight="23500" xr2:uid="{1D72018E-3503-9A41-B4B9-68ACB606B450}"/>
+    <workbookView xWindow="35840" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{1D72018E-3503-9A41-B4B9-68ACB606B450}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary_old" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="3" r:id="rId2"/>
+    <sheet name="HTSE_efficiency" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>Tech</t>
   </si>
@@ -50,12 +52,6 @@
     <t>CAPEX ($/MW)</t>
   </si>
   <si>
-    <t>FOM ($)</t>
-  </si>
-  <si>
-    <t>VOM ($)</t>
-  </si>
-  <si>
     <t>Life (y)</t>
   </si>
   <si>
@@ -72,6 +68,138 @@
   </si>
   <si>
     <t>PEM</t>
+  </si>
+  <si>
+    <t>FOM ($/MW-year)</t>
+  </si>
+  <si>
+    <t>VOM ($/MWh)</t>
+  </si>
+  <si>
+    <t>kg/s</t>
+  </si>
+  <si>
+    <t>kg/h</t>
+  </si>
+  <si>
+    <t>tpd</t>
+  </si>
+  <si>
+    <t>Module capacity</t>
+  </si>
+  <si>
+    <t>kWh/kg</t>
+  </si>
+  <si>
+    <t>MJ/kWh</t>
+  </si>
+  <si>
+    <t>MJ/kg</t>
+  </si>
+  <si>
+    <t>HHV H2</t>
+  </si>
+  <si>
+    <t>Boardman 2017, Figures of Merit</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>MSR at 700C outlet temp in Max data, point from Boardman not included</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note </t>
+  </si>
+  <si>
+    <t>HTGR</t>
+  </si>
+  <si>
+    <t>MSR</t>
+  </si>
+  <si>
+    <t>SFR</t>
+  </si>
+  <si>
+    <t>PWR</t>
+  </si>
+  <si>
+    <t>HTSE HHV efficiency</t>
+  </si>
+  <si>
+    <t>HTSE heat (MWt/kgH2)</t>
+  </si>
+  <si>
+    <t>HTSE electricity (MWe/kgH2)</t>
+  </si>
+  <si>
+    <t>Reactor type</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>H2Cap (MWe)</t>
+  </si>
+  <si>
+    <t>H2Cap (kgh2/h)</t>
+  </si>
+  <si>
+    <t>H2ElecCons (MWhe/kgh2)</t>
+  </si>
+  <si>
+    <t>H2HeatCons (MWht/kgh2)</t>
+  </si>
+  <si>
+    <t>ANR</t>
+  </si>
+  <si>
+    <t>iPWR</t>
+  </si>
+  <si>
+    <t>PBR-HTGR</t>
+  </si>
+  <si>
+    <t>iMSR</t>
+  </si>
+  <si>
+    <t>Micro</t>
+  </si>
+  <si>
+    <t>Capacity of module (kg/h)</t>
+  </si>
+  <si>
+    <t>Heat consumption (MWht/kgh2)</t>
+  </si>
+  <si>
+    <t>Electrical consumption (MWhe/kgh2)</t>
+  </si>
+  <si>
+    <t>Outlet temp</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Sodium</t>
+  </si>
+  <si>
+    <t>Fluoride Salt</t>
+  </si>
+  <si>
+    <t>Helium-cooled</t>
+  </si>
+  <si>
+    <t>Corr. To Max designs</t>
+  </si>
+  <si>
+    <t>iMSR, micro</t>
+  </si>
+  <si>
+    <t>PBR-HTGR, HTGR</t>
   </si>
 </sst>
 </file>
@@ -425,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BAD81C0-EFD6-1B4C-B7C8-767F37E93189}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,6 +562,9 @@
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -441,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -453,21 +584,27 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>25458.33</v>
+        <v>23583.3</v>
+      </c>
+      <c r="C2">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="E2">
         <v>646487</v>
@@ -484,25 +621,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>26000</v>
       </c>
       <c r="C3">
-        <v>35.299999999999997</v>
+        <v>3.5299999999999998E-2</v>
       </c>
       <c r="D3">
-        <v>9.5</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="E3">
         <v>423000</v>
       </c>
       <c r="F3">
-        <v>15943200</v>
+        <v>17218</v>
       </c>
       <c r="G3">
-        <v>10932480</v>
+        <v>1.35</v>
       </c>
       <c r="H3">
         <v>20</v>
@@ -510,12 +647,681 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>990</v>
+      </c>
+      <c r="C4">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>743865</v>
+      </c>
+      <c r="F4">
+        <v>60020</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1840.1</v>
+      </c>
+      <c r="C5">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1500000</v>
+      </c>
+      <c r="F5">
+        <v>12800</v>
+      </c>
+      <c r="G5">
+        <v>1.3</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7924EF83-4AF5-3345-AD0A-5DF9739EB424}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2">
+        <f>E2*D2</f>
+        <v>1.2699999999999998</v>
+      </c>
+      <c r="D2">
+        <f>1000/24</f>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="E2">
+        <v>3.0479999999999997E-2</v>
+      </c>
+      <c r="F2">
+        <v>8.1599999999999989E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C6" si="0">E3*D3</f>
+        <v>0.33999999999999991</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="1">1000/24</f>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="E3">
+        <v>8.1599999999999989E-3</v>
+      </c>
+      <c r="F3">
+        <v>3.1199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.33999999999999991</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="E4">
+        <v>8.1599999999999989E-3</v>
+      </c>
+      <c r="F4">
+        <v>3.1199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="E5">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="F5">
+        <v>3.024E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="E6">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="F6">
+        <v>3.024E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f>C7/E7</f>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="E7">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D11" si="2">C8/E8</f>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="E8">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="E9">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="E10">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="E11">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f>C12/E12</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="E12">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <f>C13/E13</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="E13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D13:D16" si="3">C14/E14</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="E14">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="3"/>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="E15">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="E16">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BC3F9A-E8F7-3140-B3DD-332F7878D08B}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>127</v>
+      </c>
+      <c r="C2">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>0.32</v>
+      </c>
+      <c r="E2">
+        <f>100000/24</f>
+        <v>4166.666666666667</v>
+      </c>
+      <c r="F2">
+        <f>C2/E2</f>
+        <v>8.1599999999999989E-3</v>
+      </c>
+      <c r="G2">
+        <f>B2/E2</f>
+        <v>3.0479999999999997E-2</v>
+      </c>
+      <c r="H2">
+        <v>300</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>126</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>0.45</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E5" si="0">100000/24</f>
+        <v>4166.666666666667</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F5" si="1">C3/E3</f>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G5" si="2">B3/E3</f>
+        <v>3.024E-2</v>
+      </c>
+      <c r="H3">
+        <v>550</v>
+      </c>
+      <c r="I3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>4166.666666666667</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>7.92E-3</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>2.9519999999999998E-2</v>
+      </c>
+      <c r="H4">
+        <v>850</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>130</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>0.45</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>4166.666666666667</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>8.1599999999999989E-3</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="H5">
+        <v>850</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>141.80000000000001</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>3.6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <f>B12/B13</f>
+        <v>39.388888888888893</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f>B16*1000/24</f>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <f>B17/3600</f>
+        <v>1.1574074074074073E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compute carbon intensity of hydrogen production from electricity and heat consumption and carbon intensity of nuclear energy
</commit_message>
<xml_diff>
--- a/code/h2_tech.xlsx
+++ b/code/h2_tech.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/Library/CloudStorage/OneDrive-IdahoNationalLaboratory/Documents/Research/Hydrogen from Nuclear/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\H2_ANRs\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3AA8EE-2A9F-ED47-9689-503E3324D41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C5629-D47A-4831-9FE8-8848BF831806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34640" yWindow="-440" windowWidth="27340" windowHeight="21100" activeTab="1" xr2:uid="{1D72018E-3503-9A41-B4B9-68ACB606B450}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{1D72018E-3503-9A41-B4B9-68ACB606B450}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_old" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
   <si>
     <t>Tech</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>ANR Th Eff</t>
+  </si>
+  <si>
+    <t>Carbon intensity (kgCO2eq/kgH2)</t>
+  </si>
+  <si>
+    <t>Carbon intensity ANR (kgCO2eq/MWhe)</t>
   </si>
 </sst>
 </file>
@@ -582,17 +588,17 @@
       <selection activeCell="E2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.3125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.8125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -644,7 +650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -670,7 +676,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -696,7 +702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -729,24 +735,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7924EF83-4AF5-3345-AD0A-5DF9739EB424}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.8125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.8125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -754,34 +761,40 @@
         <v>37</v>
       </c>
       <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>55</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -789,36 +802,43 @@
         <v>38</v>
       </c>
       <c r="C2">
-        <f>D2*(E2+(F2*K2))</f>
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <f>E2*(F2+(G2*L2))</f>
         <v>1.3753999999999997</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <f>1000/24</f>
         <v>41.666666666666664</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>3.0479999999999997E-2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>8.1599999999999989E-3</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>646487</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>30313.200000000001</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>2.76</v>
       </c>
-      <c r="J2" s="1">
-        <v>20</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <f>C2*(D2/E2)</f>
+        <v>0.39611519999999989</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -826,36 +846,43 @@
         <v>24</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C6" si="0">D3*(E3+(F3*K3))</f>
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="0">E3*(F3+(G3*L3))</f>
         <v>0.95099999999999985</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D6" si="1">1000/24</f>
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="1">1000/24</f>
         <v>41.666666666666664</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>8.1599999999999989E-3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>3.1199999999999999E-2</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>646487</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>30313.200000000001</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>2.76</v>
       </c>
-      <c r="J3" s="1">
-        <v>20</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <f t="shared" ref="M3:M17" si="2">C3*(D3/E3)</f>
+        <v>0.27388799999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -863,36 +890,43 @@
         <v>39</v>
       </c>
       <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
         <v>0.85999999999999988</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f t="shared" si="1"/>
         <v>41.666666666666664</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>8.1599999999999989E-3</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>3.1199999999999999E-2</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>646487</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>30313.200000000001</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2.76</v>
       </c>
-      <c r="J4" s="1">
-        <v>20</v>
-      </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>0.24767999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -900,36 +934,43 @@
         <v>40</v>
       </c>
       <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>0.89219999999999988</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="1"/>
         <v>41.666666666666664</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3.024E-2</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>646487</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>30313.200000000001</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>2.76</v>
       </c>
-      <c r="J5" s="1">
-        <v>20</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
+        <v>20</v>
+      </c>
+      <c r="L5" s="2">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>0.2569536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -937,36 +978,43 @@
         <v>41</v>
       </c>
       <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>0.71579999999999988</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f t="shared" si="1"/>
         <v>41.666666666666664</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>3.024E-2</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>646487</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>30313.200000000001</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2.76</v>
       </c>
-      <c r="J6" s="1">
-        <v>20</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>0.20615039999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -974,35 +1022,42 @@
         <v>38</v>
       </c>
       <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="D7">
-        <f>C7/E7</f>
+      <c r="E7">
+        <f>D7/F7</f>
         <v>9.9009900990099009</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.10100000000000001</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>1500000</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>12800</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1.3</v>
       </c>
-      <c r="J7" s="1">
-        <v>20</v>
-      </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
+        <v>20</v>
+      </c>
+      <c r="L7" s="2">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <f>C7*(D7/E7)</f>
+        <v>1.2120000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1010,35 +1065,42 @@
         <v>24</v>
       </c>
       <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
         <v>1</v>
       </c>
-      <c r="D8">
-        <f t="shared" ref="D8:D11" si="2">C8/E8</f>
+      <c r="E8">
+        <f t="shared" ref="E8:E11" si="3">D8/F8</f>
         <v>9.9009900990099009</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.10100000000000001</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>1500000</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>12800</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1.3</v>
       </c>
-      <c r="J8" s="1">
-        <v>20</v>
-      </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
+        <v>20</v>
+      </c>
+      <c r="L8" s="2">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>1.2120000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1046,35 +1108,42 @@
         <v>39</v>
       </c>
       <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="D9">
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="F9">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1500000</v>
+      </c>
+      <c r="I9">
+        <v>12800</v>
+      </c>
+      <c r="J9">
+        <v>1.3</v>
+      </c>
+      <c r="K9" s="1">
+        <v>20</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="2"/>
-        <v>9.9009900990099009</v>
-      </c>
-      <c r="E9">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>1500000</v>
-      </c>
-      <c r="H9">
-        <v>12800</v>
-      </c>
-      <c r="I9">
-        <v>1.3</v>
-      </c>
-      <c r="J9" s="1">
-        <v>20</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.2120000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1082,35 +1151,42 @@
         <v>40</v>
       </c>
       <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="F10">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1500000</v>
+      </c>
+      <c r="I10">
+        <v>12800</v>
+      </c>
+      <c r="J10">
+        <v>1.3</v>
+      </c>
+      <c r="K10" s="1">
+        <v>20</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="2"/>
-        <v>9.9009900990099009</v>
-      </c>
-      <c r="E10">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>1500000</v>
-      </c>
-      <c r="H10">
-        <v>12800</v>
-      </c>
-      <c r="I10">
-        <v>1.3</v>
-      </c>
-      <c r="J10" s="1">
-        <v>20</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.2120000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1118,35 +1194,42 @@
         <v>41</v>
       </c>
       <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11">
         <v>1</v>
       </c>
-      <c r="D11">
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="F11">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1500000</v>
+      </c>
+      <c r="I11">
+        <v>12800</v>
+      </c>
+      <c r="J11">
+        <v>1.3</v>
+      </c>
+      <c r="K11" s="1">
+        <v>20</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="2"/>
-        <v>9.9009900990099009</v>
-      </c>
-      <c r="E11">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>1500000</v>
-      </c>
-      <c r="H11">
-        <v>12800</v>
-      </c>
-      <c r="I11">
-        <v>1.3</v>
-      </c>
-      <c r="J11" s="1">
-        <v>20</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.2120000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1154,35 +1237,42 @@
         <v>38</v>
       </c>
       <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="D12">
-        <f>C12/E12</f>
+      <c r="E12">
+        <f>D12/F12</f>
         <v>37.037037037037038</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
       <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>743865</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>60020</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>20</v>
-      </c>
-      <c r="K12" s="2">
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>20</v>
+      </c>
+      <c r="L12" s="2">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1190,35 +1280,42 @@
         <v>24</v>
       </c>
       <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="D13">
-        <f>C13/E13</f>
+      <c r="E13">
+        <f>D13/F13</f>
         <v>37.037037037037038</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
       <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>743865</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>60020</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
-        <v>20</v>
-      </c>
-      <c r="K13" s="2">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>20</v>
+      </c>
+      <c r="L13" s="2">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1226,35 +1323,42 @@
         <v>39</v>
       </c>
       <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
         <v>2</v>
       </c>
-      <c r="D14">
-        <f>C14/E14</f>
+      <c r="E14">
+        <f>D14/F14</f>
         <v>37.037037037037038</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
       <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>743865</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>60020</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>20</v>
-      </c>
-      <c r="K14" s="2">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>20</v>
+      </c>
+      <c r="L14" s="2">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1262,35 +1366,42 @@
         <v>40</v>
       </c>
       <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="D15">
-        <f t="shared" ref="D14:D16" si="3">C15/E15</f>
+      <c r="E15">
+        <f t="shared" ref="E15:E16" si="4">D15/F15</f>
         <v>37.037037037037038</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
       <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>743865</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>60020</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>20</v>
-      </c>
-      <c r="K15" s="2">
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>20</v>
+      </c>
+      <c r="L15" s="2">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1298,32 +1409,39 @@
         <v>41</v>
       </c>
       <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="3"/>
+      <c r="E16">
+        <f t="shared" si="4"/>
         <v>37.037037037037038</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
       <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>743865</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>60020</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
-        <v>20</v>
-      </c>
-      <c r="K16" s="2">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>20</v>
+      </c>
+      <c r="L16" s="2">
         <v>0.33</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>0.64800000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1336,21 +1454,21 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.1875" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.8125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.3125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1382,7 +1500,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1417,7 +1535,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1452,7 +1570,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1484,7 +1602,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1519,7 +1637,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1527,7 +1645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1535,7 +1653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1546,7 +1664,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B13">
         <v>3.6</v>
       </c>
@@ -1554,7 +1672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
       <c r="B14">
         <f>B12/B13</f>
         <v>39.388888888888893</v>
@@ -1563,7 +1681,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1574,7 +1692,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B17">
         <f>B16*1000/24</f>
         <v>41.666666666666664</v>
@@ -1583,7 +1701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B18">
         <f>B17/3600</f>
         <v>1.1574074074074073E-2</v>

</xml_diff>

<commit_message>
add summary sheet with future htse costs
</commit_message>
<xml_diff>
--- a/code/h2_tech.xlsx
+++ b/code/h2_tech.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\H2_ANRs\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C5629-D47A-4831-9FE8-8848BF831806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B343FDF5-848F-4CFC-A44F-E8A8678C71EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{1D72018E-3503-9A41-B4B9-68ACB606B450}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="15390" windowHeight="9540" activeTab="3" xr2:uid="{1D72018E-3503-9A41-B4B9-68ACB606B450}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_old" sheetId="1" r:id="rId1"/>
-    <sheet name="Summary" sheetId="3" r:id="rId2"/>
-    <sheet name="HTSE_efficiency" sheetId="2" r:id="rId3"/>
+    <sheet name="HTSE_efficiency" sheetId="2" r:id="rId2"/>
+    <sheet name="Summary" sheetId="3" r:id="rId3"/>
+    <sheet name="Summary future HTSE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
   <si>
     <t>Tech</t>
   </si>
@@ -585,7 +586,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:G2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -734,11 +735,277 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BC3F9A-E8F7-3140-B3DD-332F7878D08B}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1875" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.8125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.3125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.3125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>127</v>
+      </c>
+      <c r="C2">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>0.32</v>
+      </c>
+      <c r="E2">
+        <f>100000/24</f>
+        <v>4166.666666666667</v>
+      </c>
+      <c r="F2">
+        <f>C2/E2</f>
+        <v>8.1599999999999989E-3</v>
+      </c>
+      <c r="G2">
+        <f>B2/E2</f>
+        <v>3.0479999999999997E-2</v>
+      </c>
+      <c r="H2">
+        <v>300</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>126</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>0.45</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E5" si="0">100000/24</f>
+        <v>4166.666666666667</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F5" si="1">C3/E3</f>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G5" si="2">B3/E3</f>
+        <v>3.024E-2</v>
+      </c>
+      <c r="H3">
+        <v>550</v>
+      </c>
+      <c r="I3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>4166.666666666667</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>7.92E-3</v>
+      </c>
+      <c r="G4">
+        <f>B4/E4</f>
+        <v>2.9519999999999998E-2</v>
+      </c>
+      <c r="H4">
+        <v>850</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>130</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>0.45</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>4166.666666666667</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>8.1599999999999989E-3</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="H5">
+        <v>850</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>141.80000000000001</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B13">
+        <v>3.6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B14">
+        <f>B12/B13</f>
+        <v>39.388888888888893</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B17">
+        <f>B16*1000/24</f>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B18">
+        <f>B17/3600</f>
+        <v>1.1574074074074073E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7924EF83-4AF5-3345-AD0A-5DF9739EB424}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -878,7 +1145,7 @@
         <v>0.47</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M17" si="2">C3*(D3/E3)</f>
+        <f t="shared" ref="M3:M16" si="2">C3*(D3/E3)</f>
         <v>0.27388799999999996</v>
       </c>
     </row>
@@ -1449,265 +1716,715 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BC3F9A-E8F7-3140-B3DD-332F7878D08B}">
-  <dimension ref="A1:J18"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8C693F-BF76-4729-941D-085939BF73D3}">
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1875" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.8125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.3125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.1875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.8125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.8125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2">
-        <v>127</v>
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
       </c>
       <c r="C2">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>0.32</v>
+        <f>E2*(F2+(G2*L2))</f>
+        <v>1.3753999999999997</v>
       </c>
       <c r="E2">
-        <f>100000/24</f>
-        <v>4166.666666666667</v>
+        <f>1000/24</f>
+        <v>41.666666666666664</v>
       </c>
       <c r="F2">
-        <f>C2/E2</f>
+        <v>3.0479999999999997E-2</v>
+      </c>
+      <c r="G2">
         <v>8.1599999999999989E-3</v>
       </c>
-      <c r="G2">
-        <f>B2/E2</f>
-        <v>3.0479999999999997E-2</v>
-      </c>
       <c r="H2">
-        <v>300</v>
-      </c>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" t="s">
+        <v>423000</v>
+      </c>
+      <c r="I2">
+        <v>17218</v>
+      </c>
+      <c r="J2">
+        <v>1.35</v>
+      </c>
+      <c r="K2" s="1">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="M2">
+        <f>C2*(D2/E2)</f>
+        <v>0.39611519999999989</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="0">E3*(F3+(G3*L3))</f>
+        <v>0.95099999999999985</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="1">1000/24</f>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="F3">
+        <v>8.1599999999999989E-3</v>
+      </c>
+      <c r="G3">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="H3">
+        <v>423000</v>
+      </c>
+      <c r="I3">
+        <v>17218</v>
+      </c>
+      <c r="J3">
+        <v>1.35</v>
+      </c>
+      <c r="K3" s="1">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M16" si="2">C3*(D3/E3)</f>
+        <v>0.27388799999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.85999999999999988</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="F4">
+        <v>8.1599999999999989E-3</v>
+      </c>
+      <c r="G4">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="H4">
+        <v>423000</v>
+      </c>
+      <c r="I4">
+        <v>17218</v>
+      </c>
+      <c r="J4">
+        <v>1.35</v>
+      </c>
+      <c r="K4" s="1">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>0.24767999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.89219999999999988</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="F5">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="G5">
+        <v>3.024E-2</v>
+      </c>
+      <c r="H5">
+        <v>423000</v>
+      </c>
+      <c r="I5">
+        <v>17218</v>
+      </c>
+      <c r="J5">
+        <v>1.35</v>
+      </c>
+      <c r="K5" s="1">
+        <v>20</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>0.2569536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.71579999999999988</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="F6">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="G6">
+        <v>3.024E-2</v>
+      </c>
+      <c r="H6">
+        <v>423000</v>
+      </c>
+      <c r="I6">
+        <v>17218</v>
+      </c>
+      <c r="J6">
+        <v>1.35</v>
+      </c>
+      <c r="K6" s="1">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>0.20615039999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3">
-        <v>126</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>0.45</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E5" si="0">100000/24</f>
-        <v>4166.666666666667</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F5" si="1">C3/E3</f>
-        <v>7.1999999999999998E-3</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G5" si="2">B3/E3</f>
-        <v>3.024E-2</v>
-      </c>
-      <c r="H3">
-        <v>550</v>
-      </c>
-      <c r="I3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4">
-        <v>123</v>
-      </c>
-      <c r="C4">
-        <v>33</v>
-      </c>
-      <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>4166.666666666667</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="1"/>
-        <v>7.92E-3</v>
-      </c>
-      <c r="G4">
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f>D7/F7</f>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="F7">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1500000</v>
+      </c>
+      <c r="I7">
+        <v>12800</v>
+      </c>
+      <c r="J7">
+        <v>1.3</v>
+      </c>
+      <c r="K7" s="1">
+        <v>20</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="M7">
+        <f>C7*(D7/E7)</f>
+        <v>1.2120000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:E11" si="3">D8/F8</f>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="F8">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1500000</v>
+      </c>
+      <c r="I8">
+        <v>12800</v>
+      </c>
+      <c r="J8">
+        <v>1.3</v>
+      </c>
+      <c r="K8" s="1">
+        <v>20</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="2"/>
-        <v>2.9519999999999998E-2</v>
-      </c>
-      <c r="H4">
-        <v>850</v>
-      </c>
-      <c r="I4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
+        <v>1.2120000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="F9">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1500000</v>
+      </c>
+      <c r="I9">
+        <v>12800</v>
+      </c>
+      <c r="J9">
+        <v>1.3</v>
+      </c>
+      <c r="K9" s="1">
+        <v>20</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>1.2120000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="F10">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1500000</v>
+      </c>
+      <c r="I10">
+        <v>12800</v>
+      </c>
+      <c r="J10">
+        <v>1.3</v>
+      </c>
+      <c r="K10" s="1">
+        <v>20</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>1.2120000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>9.9009900990099009</v>
+      </c>
+      <c r="F11">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1500000</v>
+      </c>
+      <c r="I11">
+        <v>12800</v>
+      </c>
+      <c r="J11">
+        <v>1.3</v>
+      </c>
+      <c r="K11" s="1">
+        <v>20</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>1.2120000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>D12/F12</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="F12">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>743865</v>
+      </c>
+      <c r="I12">
+        <v>60020</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>20</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="B5">
-        <v>130</v>
-      </c>
-      <c r="C5">
-        <v>34</v>
-      </c>
-      <c r="D5">
-        <v>0.45</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>4166.666666666667</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>8.1599999999999989E-3</v>
-      </c>
-      <c r="G5">
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f>D13/F13</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="F13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>743865</v>
+      </c>
+      <c r="I13">
+        <v>60020</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>20</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="2"/>
-        <v>3.1199999999999999E-2</v>
-      </c>
-      <c r="H5">
-        <v>850</v>
-      </c>
-      <c r="I5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12">
-        <v>141.80000000000001</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B13">
-        <v>3.6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B14">
-        <f>B12/B13</f>
-        <v>39.388888888888893</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <f>D14/F14</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="F14">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>743865</v>
+      </c>
+      <c r="I14">
+        <v>60020</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>20</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:E16" si="4">D15/F15</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="F15">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>743865</v>
+      </c>
+      <c r="I15">
+        <v>60020</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>20</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B17">
-        <f>B16*1000/24</f>
-        <v>41.666666666666664</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B18">
-        <f>B17/3600</f>
-        <v>1.1574074074074073E-2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="F16">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>743865</v>
+      </c>
+      <c r="I16">
+        <v>60020</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>20</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>0.64800000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compute equivalent total electricity and heat consumption for each anr-h2 coupling
</commit_message>
<xml_diff>
--- a/code/h2_tech.xlsx
+++ b/code/h2_tech.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\H2_ANRs\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B343FDF5-848F-4CFC-A44F-E8A8678C71EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0199FDF7-ED81-49B1-BD3E-F8272937D672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="15390" windowHeight="9540" activeTab="3" xr2:uid="{1D72018E-3503-9A41-B4B9-68ACB606B450}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{1D72018E-3503-9A41-B4B9-68ACB606B450}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_old" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
   <si>
     <t>Tech</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>Carbon intensity ANR (kgCO2eq/MWhe)</t>
+  </si>
+  <si>
+    <t>Eq tot H2ElecCons (MWhe/kgh2)</t>
+  </si>
+  <si>
+    <t>Eq tot H2HeatCons (MWht/kgh2)</t>
   </si>
 </sst>
 </file>
@@ -287,9 +293,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -327,7 +333,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -433,7 +439,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -575,7 +581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1002,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7924EF83-4AF5-3345-AD0A-5DF9739EB424}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1015,12 +1021,13 @@
     <col min="5" max="5" width="13.8125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.8125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="23" customWidth="1"/>
     <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1043,25 +1050,31 @@
         <v>36</v>
       </c>
       <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>56</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>57</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1072,7 +1085,7 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <f>E2*(F2+(G2*L2))</f>
+        <f>E2*(F2+(G2*N2))</f>
         <v>1.3753999999999997</v>
       </c>
       <c r="E2">
@@ -1086,26 +1099,34 @@
         <v>8.1599999999999989E-3</v>
       </c>
       <c r="H2">
+        <f>F2+G2*N2</f>
+        <v>3.3009599999999993E-2</v>
+      </c>
+      <c r="I2">
+        <f>G2+F2/N2</f>
+        <v>0.10648258064516128</v>
+      </c>
+      <c r="J2">
         <v>646487</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>30313.200000000001</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>2.76</v>
       </c>
-      <c r="K2" s="1">
-        <v>20</v>
-      </c>
-      <c r="L2" s="2">
+      <c r="M2" s="1">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2">
         <v>0.31</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <f>C2*(D2/E2)</f>
         <v>0.39611519999999989</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1116,7 +1137,7 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">E3*(F3+(G3*L3))</f>
+        <f t="shared" ref="D3:D6" si="0">E3*(F3+(G3*N3))</f>
         <v>0.95099999999999985</v>
       </c>
       <c r="E3">
@@ -1130,26 +1151,34 @@
         <v>3.1199999999999999E-2</v>
       </c>
       <c r="H3">
+        <f t="shared" ref="H3:H16" si="2">F3+G3*N3</f>
+        <v>2.2823999999999997E-2</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I16" si="3">G3+F3/N3</f>
+        <v>4.8561702127659576E-2</v>
+      </c>
+      <c r="J3">
         <v>646487</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>30313.200000000001</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>2.76</v>
       </c>
-      <c r="K3" s="1">
-        <v>20</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="M3" s="1">
+        <v>20</v>
+      </c>
+      <c r="N3" s="2">
         <v>0.47</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M16" si="2">C3*(D3/E3)</f>
+      <c r="O3">
+        <f t="shared" ref="O3:O16" si="4">C3*(D3/E3)</f>
         <v>0.27388799999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1174,26 +1203,34 @@
         <v>3.1199999999999999E-2</v>
       </c>
       <c r="H4">
+        <f t="shared" si="2"/>
+        <v>2.0639999999999999E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>5.1599999999999993E-2</v>
+      </c>
+      <c r="J4">
         <v>646487</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>30313.200000000001</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>2.76</v>
       </c>
-      <c r="K4" s="1">
-        <v>20</v>
-      </c>
-      <c r="L4" s="2">
+      <c r="M4" s="1">
+        <v>20</v>
+      </c>
+      <c r="N4" s="2">
         <v>0.4</v>
       </c>
-      <c r="M4">
-        <f t="shared" si="2"/>
+      <c r="O4">
+        <f t="shared" si="4"/>
         <v>0.24767999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1218,26 +1255,34 @@
         <v>3.024E-2</v>
       </c>
       <c r="H5">
+        <f t="shared" si="2"/>
+        <v>2.1412799999999999E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>4.5559148936170211E-2</v>
+      </c>
+      <c r="J5">
         <v>646487</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>30313.200000000001</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>2.76</v>
       </c>
-      <c r="K5" s="1">
-        <v>20</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="M5" s="1">
+        <v>20</v>
+      </c>
+      <c r="N5" s="2">
         <v>0.47</v>
       </c>
-      <c r="M5">
-        <f t="shared" si="2"/>
+      <c r="O5">
+        <f t="shared" si="4"/>
         <v>0.2569536</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1262,26 +1307,34 @@
         <v>3.024E-2</v>
       </c>
       <c r="H6">
+        <f t="shared" si="2"/>
+        <v>1.7179199999999999E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>5.2058181818181816E-2</v>
+      </c>
+      <c r="J6">
         <v>646487</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>30313.200000000001</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>2.76</v>
       </c>
-      <c r="K6" s="1">
-        <v>20</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="M6" s="1">
+        <v>20</v>
+      </c>
+      <c r="N6" s="2">
         <v>0.33</v>
       </c>
-      <c r="M6">
-        <f t="shared" si="2"/>
+      <c r="O6">
+        <f t="shared" si="4"/>
         <v>0.20615039999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1305,26 +1358,34 @@
         <v>0</v>
       </c>
       <c r="H7">
+        <f t="shared" si="2"/>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>0.32580645161290323</v>
+      </c>
+      <c r="J7">
         <v>1500000</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>12800</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>1.3</v>
       </c>
-      <c r="K7" s="1">
-        <v>20</v>
-      </c>
-      <c r="L7" s="2">
+      <c r="M7" s="1">
+        <v>20</v>
+      </c>
+      <c r="N7" s="2">
         <v>0.31</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <f>C7*(D7/E7)</f>
         <v>1.2120000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1338,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E11" si="3">D8/F8</f>
+        <f t="shared" ref="E8:E11" si="5">D8/F8</f>
         <v>9.9009900990099009</v>
       </c>
       <c r="F8">
@@ -1348,26 +1409,34 @@
         <v>0</v>
       </c>
       <c r="H8">
+        <f t="shared" si="2"/>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>0.21489361702127663</v>
+      </c>
+      <c r="J8">
         <v>1500000</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>12800</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>1.3</v>
       </c>
-      <c r="K8" s="1">
-        <v>20</v>
-      </c>
-      <c r="L8" s="2">
+      <c r="M8" s="1">
+        <v>20</v>
+      </c>
+      <c r="N8" s="2">
         <v>0.47</v>
       </c>
-      <c r="M8">
-        <f t="shared" si="2"/>
+      <c r="O8">
+        <f t="shared" si="4"/>
         <v>1.2120000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1381,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.9009900990099009</v>
       </c>
       <c r="F9">
@@ -1391,26 +1460,34 @@
         <v>0</v>
       </c>
       <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I9">
+        <f>G9+F9/N9</f>
+        <v>0.2525</v>
+      </c>
+      <c r="J9">
         <v>1500000</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>12800</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>1.3</v>
       </c>
-      <c r="K9" s="1">
-        <v>20</v>
-      </c>
-      <c r="L9" s="2">
+      <c r="M9" s="1">
+        <v>20</v>
+      </c>
+      <c r="N9" s="2">
         <v>0.4</v>
       </c>
-      <c r="M9">
-        <f t="shared" si="2"/>
+      <c r="O9">
+        <f t="shared" si="4"/>
         <v>1.2120000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1424,7 +1501,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.9009900990099009</v>
       </c>
       <c r="F10">
@@ -1434,26 +1511,34 @@
         <v>0</v>
       </c>
       <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>0.21489361702127663</v>
+      </c>
+      <c r="J10">
         <v>1500000</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>12800</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>1.3</v>
       </c>
-      <c r="K10" s="1">
-        <v>20</v>
-      </c>
-      <c r="L10" s="2">
+      <c r="M10" s="1">
+        <v>20</v>
+      </c>
+      <c r="N10" s="2">
         <v>0.47</v>
       </c>
-      <c r="M10">
-        <f t="shared" si="2"/>
+      <c r="O10">
+        <f t="shared" si="4"/>
         <v>1.2120000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1467,7 +1552,7 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.9009900990099009</v>
       </c>
       <c r="F11">
@@ -1477,26 +1562,34 @@
         <v>0</v>
       </c>
       <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>0.30606060606060609</v>
+      </c>
+      <c r="J11">
         <v>1500000</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>12800</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>1.3</v>
       </c>
-      <c r="K11" s="1">
-        <v>20</v>
-      </c>
-      <c r="L11" s="2">
+      <c r="M11" s="1">
+        <v>20</v>
+      </c>
+      <c r="N11" s="2">
         <v>0.33</v>
       </c>
-      <c r="M11">
-        <f t="shared" si="2"/>
+      <c r="O11">
+        <f t="shared" si="4"/>
         <v>1.2120000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1520,26 +1613,34 @@
         <v>0</v>
       </c>
       <c r="H12">
+        <f t="shared" si="2"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>0.17419354838709677</v>
+      </c>
+      <c r="J12">
         <v>743865</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>60020</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>20</v>
-      </c>
-      <c r="L12" s="2">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>20</v>
+      </c>
+      <c r="N12" s="2">
         <v>0.31</v>
       </c>
-      <c r="M12">
-        <f t="shared" si="2"/>
+      <c r="O12">
+        <f t="shared" si="4"/>
         <v>0.64800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1563,26 +1664,34 @@
         <v>0</v>
       </c>
       <c r="H13">
+        <f t="shared" si="2"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>0.1148936170212766</v>
+      </c>
+      <c r="J13">
         <v>743865</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>60020</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>20</v>
-      </c>
-      <c r="L13" s="2">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>20</v>
+      </c>
+      <c r="N13" s="2">
         <v>0.47</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="2"/>
+      <c r="O13">
+        <f t="shared" si="4"/>
         <v>0.64800000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1606,26 +1715,34 @@
         <v>0</v>
       </c>
       <c r="H14">
+        <f t="shared" si="2"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>0.13499999999999998</v>
+      </c>
+      <c r="J14">
         <v>743865</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>60020</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1">
-        <v>20</v>
-      </c>
-      <c r="L14" s="2">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>20</v>
+      </c>
+      <c r="N14" s="2">
         <v>0.4</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
+      <c r="O14">
+        <f t="shared" si="4"/>
         <v>0.64800000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1639,7 +1756,7 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E15:E16" si="4">D15/F15</f>
+        <f t="shared" ref="E15:E16" si="6">D15/F15</f>
         <v>37.037037037037038</v>
       </c>
       <c r="F15">
@@ -1649,26 +1766,34 @@
         <v>0</v>
       </c>
       <c r="H15">
+        <f t="shared" si="2"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>0.1148936170212766</v>
+      </c>
+      <c r="J15">
         <v>743865</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>60020</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>20</v>
-      </c>
-      <c r="L15" s="2">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>20</v>
+      </c>
+      <c r="N15" s="2">
         <v>0.47</v>
       </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
+      <c r="O15">
+        <f t="shared" si="4"/>
         <v>0.64800000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1682,7 +1807,7 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37.037037037037038</v>
       </c>
       <c r="F16">
@@ -1692,22 +1817,30 @@
         <v>0</v>
       </c>
       <c r="H16">
+        <f t="shared" si="2"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>0.16363636363636364</v>
+      </c>
+      <c r="J16">
         <v>743865</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>60020</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
-        <v>20</v>
-      </c>
-      <c r="L16" s="2">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>20</v>
+      </c>
+      <c r="N16" s="2">
         <v>0.33</v>
       </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
+      <c r="O16">
+        <f t="shared" si="4"/>
         <v>0.64800000000000002</v>
       </c>
     </row>
@@ -1720,7 +1853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8C693F-BF76-4729-941D-085939BF73D3}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add carbon intensity from LCA ANL analysis
</commit_message>
<xml_diff>
--- a/code/h2_tech.xlsx
+++ b/code/h2_tech.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\H2_ANRs\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0199FDF7-ED81-49B1-BD3E-F8272937D672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2486B270-ED9A-4901-BC0C-2CD4EF8C1826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{1D72018E-3503-9A41-B4B9-68ACB606B450}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{1D72018E-3503-9A41-B4B9-68ACB606B450}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_old" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
   <si>
     <t>Tech</t>
   </si>
@@ -1008,26 +1008,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7924EF83-4AF5-3345-AD0A-5DF9739EB424}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="3" max="3" width="32.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.8125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.8125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.8125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.8125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1035,46 +1034,43 @@
         <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="H1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="M1" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="N1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1082,51 +1078,47 @@
         <v>38</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <f>D2*(E2+(F2*M2))</f>
+        <v>1.3753999999999997</v>
       </c>
       <c r="D2">
-        <f>E2*(F2+(G2*N2))</f>
-        <v>1.3753999999999997</v>
-      </c>
-      <c r="E2">
         <f>1000/24</f>
         <v>41.666666666666664</v>
       </c>
+      <c r="E2">
+        <v>3.0479999999999997E-2</v>
+      </c>
       <c r="F2">
-        <v>3.0479999999999997E-2</v>
+        <v>8.1599999999999989E-3</v>
       </c>
       <c r="G2">
-        <v>8.1599999999999989E-3</v>
+        <f>E2+F2*M2</f>
+        <v>3.3009599999999993E-2</v>
       </c>
       <c r="H2">
-        <f>F2+G2*N2</f>
-        <v>3.3009599999999993E-2</v>
+        <f>F2+E2/M2</f>
+        <v>0.10648258064516128</v>
       </c>
       <c r="I2">
-        <f>G2+F2/N2</f>
-        <v>0.10648258064516128</v>
+        <v>646487</v>
       </c>
       <c r="J2">
-        <v>646487</v>
+        <v>30313.200000000001</v>
       </c>
       <c r="K2">
-        <v>30313.200000000001</v>
-      </c>
-      <c r="L2">
         <v>2.76</v>
       </c>
-      <c r="M2" s="1">
-        <v>20</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="L2" s="1">
+        <v>20</v>
+      </c>
+      <c r="M2" s="2">
         <v>0.31</v>
       </c>
-      <c r="O2">
-        <f>C2*(D2/E2)</f>
-        <v>0.39611519999999989</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1134,51 +1126,47 @@
         <v>24</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <f t="shared" ref="C3:C6" si="0">D3*(E3+(F3*M3))</f>
+        <v>0.95099999999999985</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">E3*(F3+(G3*N3))</f>
-        <v>0.95099999999999985</v>
+        <f t="shared" ref="D3:D6" si="1">1000/24</f>
+        <v>41.666666666666664</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E6" si="1">1000/24</f>
-        <v>41.666666666666664</v>
+        <v>8.1599999999999989E-3</v>
       </c>
       <c r="F3">
-        <v>8.1599999999999989E-3</v>
+        <v>3.1199999999999999E-2</v>
       </c>
       <c r="G3">
-        <v>3.1199999999999999E-2</v>
+        <f t="shared" ref="G3:G16" si="2">E3+F3*M3</f>
+        <v>2.2823999999999997E-2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H16" si="2">F3+G3*N3</f>
-        <v>2.2823999999999997E-2</v>
+        <f t="shared" ref="H3:H16" si="3">F3+E3/M3</f>
+        <v>4.8561702127659576E-2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I16" si="3">G3+F3/N3</f>
-        <v>4.8561702127659576E-2</v>
+        <v>646487</v>
       </c>
       <c r="J3">
-        <v>646487</v>
+        <v>30313.200000000001</v>
       </c>
       <c r="K3">
-        <v>30313.200000000001</v>
-      </c>
-      <c r="L3">
         <v>2.76</v>
       </c>
-      <c r="M3" s="1">
-        <v>20</v>
-      </c>
-      <c r="N3" s="2">
+      <c r="L3" s="1">
+        <v>20</v>
+      </c>
+      <c r="M3" s="2">
         <v>0.47</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O16" si="4">C3*(D3/E3)</f>
-        <v>0.27388799999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1186,51 +1174,47 @@
         <v>39</v>
       </c>
       <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
         <f t="shared" si="0"/>
         <v>0.85999999999999988</v>
       </c>
-      <c r="E4">
+      <c r="D4">
         <f t="shared" si="1"/>
         <v>41.666666666666664</v>
       </c>
+      <c r="E4">
+        <v>8.1599999999999989E-3</v>
+      </c>
       <c r="F4">
-        <v>8.1599999999999989E-3</v>
+        <v>3.1199999999999999E-2</v>
       </c>
       <c r="G4">
-        <v>3.1199999999999999E-2</v>
-      </c>
-      <c r="H4">
         <f t="shared" si="2"/>
         <v>2.0639999999999999E-2</v>
       </c>
-      <c r="I4">
+      <c r="H4">
         <f t="shared" si="3"/>
         <v>5.1599999999999993E-2</v>
       </c>
+      <c r="I4">
+        <v>646487</v>
+      </c>
       <c r="J4">
-        <v>646487</v>
+        <v>30313.200000000001</v>
       </c>
       <c r="K4">
-        <v>30313.200000000001</v>
-      </c>
-      <c r="L4">
         <v>2.76</v>
       </c>
-      <c r="M4" s="1">
-        <v>20</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="L4" s="1">
+        <v>20</v>
+      </c>
+      <c r="M4" s="2">
         <v>0.4</v>
       </c>
-      <c r="O4">
-        <f t="shared" si="4"/>
-        <v>0.24767999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1238,51 +1222,47 @@
         <v>40</v>
       </c>
       <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
         <f t="shared" si="0"/>
         <v>0.89219999999999988</v>
       </c>
-      <c r="E5">
+      <c r="D5">
         <f t="shared" si="1"/>
         <v>41.666666666666664</v>
       </c>
+      <c r="E5">
+        <v>7.1999999999999998E-3</v>
+      </c>
       <c r="F5">
-        <v>7.1999999999999998E-3</v>
+        <v>3.024E-2</v>
       </c>
       <c r="G5">
-        <v>3.024E-2</v>
-      </c>
-      <c r="H5">
         <f t="shared" si="2"/>
         <v>2.1412799999999999E-2</v>
       </c>
-      <c r="I5">
+      <c r="H5">
         <f t="shared" si="3"/>
         <v>4.5559148936170211E-2</v>
       </c>
+      <c r="I5">
+        <v>646487</v>
+      </c>
       <c r="J5">
-        <v>646487</v>
+        <v>30313.200000000001</v>
       </c>
       <c r="K5">
-        <v>30313.200000000001</v>
-      </c>
-      <c r="L5">
         <v>2.76</v>
       </c>
-      <c r="M5" s="1">
-        <v>20</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="L5" s="1">
+        <v>20</v>
+      </c>
+      <c r="M5" s="2">
         <v>0.47</v>
       </c>
-      <c r="O5">
-        <f t="shared" si="4"/>
-        <v>0.2569536</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1290,51 +1270,47 @@
         <v>41</v>
       </c>
       <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6">
         <f t="shared" si="0"/>
         <v>0.71579999999999988</v>
       </c>
-      <c r="E6">
+      <c r="D6">
         <f t="shared" si="1"/>
         <v>41.666666666666664</v>
       </c>
+      <c r="E6">
+        <v>7.1999999999999998E-3</v>
+      </c>
       <c r="F6">
-        <v>7.1999999999999998E-3</v>
+        <v>3.024E-2</v>
       </c>
       <c r="G6">
-        <v>3.024E-2</v>
-      </c>
-      <c r="H6">
         <f t="shared" si="2"/>
         <v>1.7179199999999999E-2</v>
       </c>
-      <c r="I6">
+      <c r="H6">
         <f t="shared" si="3"/>
         <v>5.2058181818181816E-2</v>
       </c>
+      <c r="I6">
+        <v>646487</v>
+      </c>
       <c r="J6">
-        <v>646487</v>
+        <v>30313.200000000001</v>
       </c>
       <c r="K6">
-        <v>30313.200000000001</v>
-      </c>
-      <c r="L6">
         <v>2.76</v>
       </c>
-      <c r="M6" s="1">
-        <v>20</v>
-      </c>
-      <c r="N6" s="2">
+      <c r="L6" s="1">
+        <v>20</v>
+      </c>
+      <c r="M6" s="2">
         <v>0.33</v>
       </c>
-      <c r="O6">
-        <f t="shared" si="4"/>
-        <v>0.20615039999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1342,50 +1318,46 @@
         <v>38</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <f>C7/E7</f>
+        <v>9.9009900990099009</v>
       </c>
       <c r="E7">
-        <f>D7/F7</f>
-        <v>9.9009900990099009</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F7">
-        <v>0.10100000000000001</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
         <f t="shared" si="2"/>
         <v>0.10100000000000001</v>
       </c>
-      <c r="I7">
+      <c r="H7">
         <f t="shared" si="3"/>
         <v>0.32580645161290323</v>
       </c>
+      <c r="I7">
+        <v>1500000</v>
+      </c>
       <c r="J7">
-        <v>1500000</v>
+        <v>12800</v>
       </c>
       <c r="K7">
-        <v>12800</v>
-      </c>
-      <c r="L7">
         <v>1.3</v>
       </c>
-      <c r="M7" s="1">
-        <v>20</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="L7" s="1">
+        <v>20</v>
+      </c>
+      <c r="M7" s="2">
         <v>0.31</v>
       </c>
-      <c r="O7">
-        <f>C7*(D7/E7)</f>
-        <v>1.2120000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1393,50 +1365,46 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <f t="shared" ref="D8:D11" si="4">C8/E8</f>
+        <v>9.9009900990099009</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E11" si="5">D8/F8</f>
-        <v>9.9009900990099009</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F8">
-        <v>0.10100000000000001</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
         <f t="shared" si="2"/>
         <v>0.10100000000000001</v>
       </c>
-      <c r="I8">
+      <c r="H8">
         <f t="shared" si="3"/>
         <v>0.21489361702127663</v>
       </c>
+      <c r="I8">
+        <v>1500000</v>
+      </c>
       <c r="J8">
-        <v>1500000</v>
+        <v>12800</v>
       </c>
       <c r="K8">
-        <v>12800</v>
-      </c>
-      <c r="L8">
         <v>1.3</v>
       </c>
-      <c r="M8" s="1">
-        <v>20</v>
-      </c>
-      <c r="N8" s="2">
+      <c r="L8" s="1">
+        <v>20</v>
+      </c>
+      <c r="M8" s="2">
         <v>0.47</v>
       </c>
-      <c r="O8">
-        <f t="shared" si="4"/>
-        <v>1.2120000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1444,50 +1412,46 @@
         <v>39</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>9.9009900990099009</v>
       </c>
       <c r="E9">
-        <f t="shared" si="5"/>
-        <v>9.9009900990099009</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F9">
-        <v>0.10100000000000001</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
         <f t="shared" si="2"/>
         <v>0.10100000000000001</v>
       </c>
+      <c r="H9">
+        <f>F9+E9/M9</f>
+        <v>0.2525</v>
+      </c>
       <c r="I9">
-        <f>G9+F9/N9</f>
-        <v>0.2525</v>
+        <v>1500000</v>
       </c>
       <c r="J9">
-        <v>1500000</v>
+        <v>12800</v>
       </c>
       <c r="K9">
-        <v>12800</v>
-      </c>
-      <c r="L9">
         <v>1.3</v>
       </c>
-      <c r="M9" s="1">
-        <v>20</v>
-      </c>
-      <c r="N9" s="2">
+      <c r="L9" s="1">
+        <v>20</v>
+      </c>
+      <c r="M9" s="2">
         <v>0.4</v>
       </c>
-      <c r="O9">
-        <f t="shared" si="4"/>
-        <v>1.2120000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1495,50 +1459,46 @@
         <v>40</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>9.9009900990099009</v>
       </c>
       <c r="E10">
-        <f t="shared" si="5"/>
-        <v>9.9009900990099009</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F10">
-        <v>0.10100000000000001</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
         <f t="shared" si="2"/>
         <v>0.10100000000000001</v>
       </c>
-      <c r="I10">
+      <c r="H10">
         <f t="shared" si="3"/>
         <v>0.21489361702127663</v>
       </c>
+      <c r="I10">
+        <v>1500000</v>
+      </c>
       <c r="J10">
-        <v>1500000</v>
+        <v>12800</v>
       </c>
       <c r="K10">
-        <v>12800</v>
-      </c>
-      <c r="L10">
         <v>1.3</v>
       </c>
-      <c r="M10" s="1">
-        <v>20</v>
-      </c>
-      <c r="N10" s="2">
+      <c r="L10" s="1">
+        <v>20</v>
+      </c>
+      <c r="M10" s="2">
         <v>0.47</v>
       </c>
-      <c r="O10">
-        <f t="shared" si="4"/>
-        <v>1.2120000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1546,50 +1506,46 @@
         <v>41</v>
       </c>
       <c r="C11">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>9.9009900990099009</v>
       </c>
       <c r="E11">
-        <f t="shared" si="5"/>
-        <v>9.9009900990099009</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F11">
-        <v>0.10100000000000001</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
         <f t="shared" si="2"/>
         <v>0.10100000000000001</v>
       </c>
-      <c r="I11">
+      <c r="H11">
         <f t="shared" si="3"/>
         <v>0.30606060606060609</v>
       </c>
+      <c r="I11">
+        <v>1500000</v>
+      </c>
       <c r="J11">
-        <v>1500000</v>
+        <v>12800</v>
       </c>
       <c r="K11">
-        <v>12800</v>
-      </c>
-      <c r="L11">
         <v>1.3</v>
       </c>
-      <c r="M11" s="1">
-        <v>20</v>
-      </c>
-      <c r="N11" s="2">
+      <c r="L11" s="1">
+        <v>20</v>
+      </c>
+      <c r="M11" s="2">
         <v>0.33</v>
       </c>
-      <c r="O11">
-        <f t="shared" si="4"/>
-        <v>1.2120000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1597,50 +1553,46 @@
         <v>38</v>
       </c>
       <c r="C12">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <f>C12/E12</f>
+        <v>37.037037037037038</v>
       </c>
       <c r="E12">
-        <f>D12/F12</f>
-        <v>37.037037037037038</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="F12">
-        <v>5.3999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
         <f t="shared" si="2"/>
         <v>5.3999999999999999E-2</v>
       </c>
+      <c r="H12">
+        <f>F12+E12/M12</f>
+        <v>0.17419354838709677</v>
+      </c>
       <c r="I12">
-        <f t="shared" si="3"/>
-        <v>0.17419354838709677</v>
+        <v>743865</v>
       </c>
       <c r="J12">
-        <v>743865</v>
+        <v>60020</v>
       </c>
       <c r="K12">
-        <v>60020</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="1">
-        <v>20</v>
-      </c>
-      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>20</v>
+      </c>
+      <c r="M12" s="2">
         <v>0.31</v>
       </c>
-      <c r="O12">
-        <f t="shared" si="4"/>
-        <v>0.64800000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1648,200 +1600,184 @@
         <v>24</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D13">
+        <f>C13/E13</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="E13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>E13+F13*M13</f>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>0.1148936170212766</v>
+      </c>
+      <c r="I13">
+        <v>743865</v>
+      </c>
+      <c r="J13">
+        <v>60020</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>20</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="N13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
         <v>2</v>
       </c>
-      <c r="E13">
-        <f>D13/F13</f>
+      <c r="D14">
+        <f>C14/E14</f>
         <v>37.037037037037038</v>
       </c>
-      <c r="F13">
+      <c r="E14">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="2"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="I13">
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>0.13499999999999998</v>
+      </c>
+      <c r="I14">
+        <v>743865</v>
+      </c>
+      <c r="J14">
+        <v>60020</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>20</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="N14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:D16" si="5">C15/E15</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="E15">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="3"/>
         <v>0.1148936170212766</v>
       </c>
-      <c r="J13">
+      <c r="I15">
         <v>743865</v>
       </c>
-      <c r="K13">
+      <c r="J15">
         <v>60020</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1">
-        <v>20</v>
-      </c>
-      <c r="N13" s="2">
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>20</v>
+      </c>
+      <c r="M15" s="2">
         <v>0.47</v>
       </c>
-      <c r="O13">
-        <f t="shared" si="4"/>
-        <v>0.64800000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A14" t="s">
+      <c r="N15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14">
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
         <v>2</v>
       </c>
-      <c r="E14">
-        <f>D14/F14</f>
+      <c r="D16">
+        <f t="shared" si="5"/>
         <v>37.037037037037038</v>
       </c>
-      <c r="F14">
+      <c r="E16">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="2"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="3"/>
-        <v>0.13499999999999998</v>
-      </c>
-      <c r="J14">
-        <v>743865</v>
-      </c>
-      <c r="K14">
-        <v>60020</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" s="1">
-        <v>20</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="4"/>
-        <v>0.64800000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15">
-        <v>12</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <f t="shared" ref="E15:E16" si="6">D15/F15</f>
-        <v>37.037037037037038</v>
-      </c>
-      <c r="F15">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="3"/>
-        <v>0.1148936170212766</v>
-      </c>
-      <c r="J15">
-        <v>743865</v>
-      </c>
-      <c r="K15">
-        <v>60020</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="1">
-        <v>20</v>
-      </c>
-      <c r="N15" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="4"/>
-        <v>0.64800000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16">
-        <v>12</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="6"/>
-        <v>37.037037037037038</v>
-      </c>
-      <c r="F16">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
       <c r="H16">
-        <f t="shared" si="2"/>
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="I16">
         <f t="shared" si="3"/>
         <v>0.16363636363636364</v>
       </c>
+      <c r="I16">
+        <v>743865</v>
+      </c>
       <c r="J16">
-        <v>743865</v>
+        <v>60020</v>
       </c>
       <c r="K16">
-        <v>60020</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1">
-        <v>20</v>
-      </c>
-      <c r="N16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>20</v>
+      </c>
+      <c r="M16" s="2">
         <v>0.33</v>
       </c>
-      <c r="O16">
-        <f t="shared" si="4"/>
-        <v>0.64800000000000002</v>
+      <c r="N16">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>